<commit_message>
clinic add pages updated
</commit_message>
<xml_diff>
--- a/public/uploads/test.xlsx
+++ b/public/uploads/test.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Full Liste" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="deneme" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Full Liste'!$A$1:$L$721</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">deneme!$A$1:$L$721</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
@@ -15,40 +15,40 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5988" uniqueCount="3523">
   <si>
-    <t>contactInformation[details]</t>
-  </si>
-  <si>
-    <t>companyInformation[companyName]</t>
-  </si>
-  <si>
-    <t>adress[zipCode]</t>
-  </si>
-  <si>
-    <t>address[country]</t>
-  </si>
-  <si>
-    <t>address[city]</t>
-  </si>
-  <si>
-    <t>address[district]</t>
-  </si>
-  <si>
-    <t>address[adressDetailText]</t>
-  </si>
-  <si>
-    <t>contactInformation[phone]</t>
-  </si>
-  <si>
-    <t>personalInformation[email]</t>
-  </si>
-  <si>
-    <t>centerDetails[centerType]</t>
-  </si>
-  <si>
-    <t>companyInformation[photo]</t>
-  </si>
-  <si>
-    <t>companyInformation[bio]</t>
+    <t>number</t>
+  </si>
+  <si>
+    <t>companyName</t>
+  </si>
+  <si>
+    <t>zipCode</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>adressDetailText</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>centerType</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>bio</t>
   </si>
   <si>
     <t>ÖZEL FMC ATAŞEHİR DİYALİZ MERKEZİ</t>
@@ -11822,10 +11822,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>

</xml_diff>